<commit_message>
Updated notebooks and datasets
</commit_message>
<xml_diff>
--- a/GWR Outputs/GWR with SAMHI.xlsx
+++ b/GWR Outputs/GWR with SAMHI.xlsx
@@ -34,10 +34,21 @@
     <sheet name="Model 1 Parameters Summary" sheetId="24" r:id="rId24"/>
     <sheet name="Model 1_Sig" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>

<commit_message>
Updated code and datasets
</commit_message>
<xml_diff>
--- a/GWR Outputs/GWR with SAMHI.xlsx
+++ b/GWR Outputs/GWR with SAMHI.xlsx
@@ -29,6 +29,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sig_RUC_SD" sheetId="21" state="visible" r:id="rId21"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sig_RUC_FFF" sheetId="22" state="visible" r:id="rId22"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sig_RUC_E_Comm" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model 1 Parameters Summary" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model 1_Sig" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -25835,6 +25837,292 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>STD</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Median</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5.711</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.632</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.011</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5.722</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Combined Decile</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.217</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.233</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.079</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-0.168</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.485</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>LSOA_Count</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Median</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Total_LSOAs</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>LSOA_Coverage</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cherwell</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>38</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.336</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.296</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.629</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-0.259</v>
+      </c>
+      <c r="H2" t="n">
+        <v>102</v>
+      </c>
+      <c r="I2" t="n">
+        <v>37.255</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Oxford</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>51</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.621</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.545</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1.079</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-0.298</v>
+      </c>
+      <c r="H3" t="n">
+        <v>85</v>
+      </c>
+      <c r="I3" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>South Oxfordshire</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>32</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.475</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.463</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.795</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.344</v>
+      </c>
+      <c r="H4" t="n">
+        <v>93</v>
+      </c>
+      <c r="I4" t="n">
+        <v>34.409</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>West Oxfordshire</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.433</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="H5" t="n">
+        <v>68</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5.882</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>